<commit_message>
Experiment uitgevoerd en waarden genoteerd in python en in excel
</commit_message>
<xml_diff>
--- a/IE1_metingen_raw.xlsx
+++ b/IE1_metingen_raw.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpols\surfdrive\Onderwijs\1e jaars practicum\Experimenten\01 IE 1\Documenten\Labjournal opdracht\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenna\PycharmProjects\practicum131023\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E6E9E8-11C0-40FC-816F-929E418D0197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>h12_afstotend</t>
-  </si>
-  <si>
     <t>F12_afstotend</t>
   </si>
   <si>
@@ -43,11 +41,14 @@
   <si>
     <t>m12_aantrekkend</t>
   </si>
+  <si>
+    <t>h12_afstotend (mm)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,14 +359,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
@@ -373,24 +374,164 @@
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="D2">
+        <v>47</v>
+      </c>
+      <c r="E2">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="D4">
+        <v>11.5</v>
+      </c>
+      <c r="E4">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>0.114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>0.13600000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>10.5</v>
+      </c>
+      <c r="B8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>0.153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>2.7E-2</v>
+      </c>
+      <c r="D9">
+        <v>5.2</v>
+      </c>
+      <c r="E9">
+        <v>0.187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D10">
+        <v>4.7</v>
+      </c>
+      <c r="E10">
+        <v>0.20799999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>8.5</v>
+      </c>
+      <c r="B11">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>0.245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>